<commit_message>
Computation of Pressure Drop on First echelon
</commit_message>
<xml_diff>
--- a/src/data/toy_problem.xlsx
+++ b/src/data/toy_problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\ExxonMobil\LM_Gathering\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41663FB-EAE2-4C49-B4C6-BD69CC962573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CFF933-CAB8-42D1-A049-3F18DD8A5CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="215">
   <si>
     <t>Parameter</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Start-time</t>
   </si>
   <si>
-    <t>Oil Production [BBL/day]</t>
-  </si>
-  <si>
     <t>pf3</t>
   </si>
   <si>
@@ -683,6 +680,15 @@
   </si>
   <si>
     <t>t120</t>
+  </si>
+  <si>
+    <t>Gas production [mscf/day]</t>
+  </si>
+  <si>
+    <t>Oil production [BBL/day]</t>
+  </si>
+  <si>
+    <t>Water production [BBL/day]</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4831190-D3FC-4651-BCE2-3D00A10B68E5}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
@@ -1190,7 +1196,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>54</v>
@@ -1219,7 +1225,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>55</v>
@@ -1239,14 +1245,14 @@
         <v>38</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>56</v>
@@ -1271,7 +1277,7 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="8" t="s">
@@ -1292,7 +1298,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="8"/>
       <c r="I6" s="8" t="s">
@@ -1313,7 +1319,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="8"/>
       <c r="I7" s="8" t="s">
@@ -1334,7 +1340,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="8"/>
       <c r="I8" s="8" t="s">
@@ -1355,7 +1361,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="8"/>
       <c r="I9" s="8" t="s">
@@ -1376,7 +1382,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="8"/>
       <c r="I10" s="8" t="s">
@@ -1397,7 +1403,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="8"/>
       <c r="I11" s="8" t="s">
@@ -1418,7 +1424,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12" s="8"/>
       <c r="I12" s="8" t="s">
@@ -1439,7 +1445,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" s="8"/>
       <c r="I13" s="8" t="s">
@@ -1456,7 +1462,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="8"/>
       <c r="I14" s="8" t="s">
@@ -1473,7 +1479,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="8"/>
       <c r="I15" s="8" t="s">
@@ -1490,7 +1496,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="8"/>
       <c r="I16" s="8" t="s">
@@ -1507,7 +1513,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G17" s="8"/>
       <c r="I17" s="8" t="s">
@@ -1524,7 +1530,7 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" s="8"/>
       <c r="I18" s="8" t="s">
@@ -1541,7 +1547,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="8"/>
       <c r="I19" s="8" t="s">
@@ -1558,7 +1564,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" s="8"/>
       <c r="I20" s="8" t="s">
@@ -1575,7 +1581,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="8"/>
       <c r="I21" s="8" t="s">
@@ -1592,7 +1598,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G22" s="8"/>
       <c r="I22" s="8" t="s">
@@ -1609,7 +1615,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="8"/>
       <c r="I23" s="8" t="s">
@@ -1626,7 +1632,7 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G24" s="8"/>
       <c r="I24" s="8" t="s">
@@ -1643,7 +1649,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G25" s="8"/>
       <c r="I25" s="8" t="s">
@@ -1660,7 +1666,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="8"/>
       <c r="I26" s="8" t="s">
@@ -1677,7 +1683,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G27" s="8"/>
       <c r="I27" s="8" t="s">
@@ -1694,7 +1700,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28" s="8"/>
       <c r="I28" s="8" t="s">
@@ -1711,7 +1717,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="8"/>
       <c r="I29" s="8" t="s">
@@ -1728,7 +1734,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G30" s="8"/>
       <c r="I30" s="8" t="s">
@@ -1745,7 +1751,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G31" s="8"/>
       <c r="I31" s="8" t="s">
@@ -1762,7 +1768,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" s="8"/>
       <c r="I32" s="8" t="s">
@@ -1779,7 +1785,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="8"/>
       <c r="I33" s="8" t="s">
@@ -1796,7 +1802,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" s="8"/>
       <c r="I34" s="8" t="s">
@@ -1813,7 +1819,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" s="8"/>
       <c r="I35" s="8" t="s">
@@ -1830,7 +1836,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" s="8"/>
       <c r="I36" s="8" t="s">
@@ -1847,7 +1853,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G37" s="8"/>
       <c r="I37" s="8" t="s">
@@ -1864,7 +1870,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G38" s="8"/>
       <c r="I38" s="8"/>
@@ -1877,7 +1883,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G39" s="8"/>
       <c r="I39" s="8"/>
@@ -1890,7 +1896,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G40" s="8"/>
       <c r="I40" s="8"/>
@@ -1903,7 +1909,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G41" s="8"/>
       <c r="I41" s="8"/>
@@ -1916,7 +1922,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G42" s="8"/>
       <c r="I42" s="8"/>
@@ -1929,7 +1935,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G43" s="8"/>
       <c r="I43" s="8"/>
@@ -1942,7 +1948,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44" s="8"/>
       <c r="I44" s="8"/>
@@ -1955,7 +1961,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45" s="8"/>
       <c r="I45" s="8"/>
@@ -1968,7 +1974,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G46" s="8"/>
       <c r="I46" s="8"/>
@@ -1981,7 +1987,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G47" s="8"/>
       <c r="I47" s="8"/>
@@ -1994,7 +2000,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G48" s="8"/>
       <c r="I48" s="8"/>
@@ -2002,367 +2008,367 @@
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F55" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F62" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F63" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F64" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F80" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="107" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F107" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F108" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="109" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F109" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="110" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F110" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F111" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F112" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F113" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F114" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F115" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="116" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F116" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F117" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="118" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F118" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F119" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F120" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F121" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +2967,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
@@ -3000,10 +3006,10 @@
         <v>47</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R1" t="s">
         <v>48</v>
@@ -3619,1090 +3625,2058 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEBBF0F-EABE-44EA-8F33-9EEF8F969E25}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="7">
         <v>6500</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="7">
+        <f>B2*2</f>
+        <v>13000</v>
+      </c>
+      <c r="D2" s="7">
+        <f>B2*3.5</f>
+        <v>22750</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="20"/>
+      <c r="I2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="7">
+      <c r="J2" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="7">
         <v>6100</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C66" si="0">B3*2</f>
+        <v>12200</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D66" si="1">B3*3.5</f>
+        <v>21350</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7">
+      <c r="J3" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="7">
         <v>5200</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>10400</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="1"/>
+        <v>18200</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="7">
+      <c r="J4" s="7">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="7">
         <v>4400</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>8800</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
+        <v>15400</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="7">
+      <c r="J5" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="7">
         <v>4000</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>14000</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="7">
+      <c r="J6" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="7">
         <v>3700</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>7400</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>12950</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="7">
+      <c r="J7" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="7">
         <v>3400</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>6800</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>11900</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="7">
+      <c r="J8" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="7">
         <v>3200</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>6400</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>11200</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="7">
+      <c r="J9" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="7">
         <v>3000</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>10500</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="7">
+      <c r="J10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="7">
         <v>2800</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>5600</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>9800</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="7">
+      <c r="J11" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="7">
         <v>2600</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>5200</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>9100</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="7">
+      <c r="J12" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="7">
         <v>2400</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>8400</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="7">
+      <c r="J13" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="7">
         <v>2260</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>4520</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>7910</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="7">
         <v>2110</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>4220</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>7385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="7">
         <v>1970</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>3940</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>6895</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="7">
         <v>1850</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>3700</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>6475</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="7">
         <v>1730</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>3460</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>6055</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" s="7">
         <v>1610</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>3220</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
+        <v>5635</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="7">
         <v>1510</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>3020</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>5285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="7">
         <v>1410</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>2820</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
+        <v>4935</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="7">
         <v>1320</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="7">
+        <f t="shared" si="0"/>
+        <v>2640</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" s="7">
         <v>1230</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>2460</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="1"/>
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="7">
         <v>1160</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>2320</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="1"/>
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="7">
         <v>1090</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
+        <v>2180</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="1"/>
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="7">
         <v>1030</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
+        <v>2060</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="1"/>
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="7">
         <v>972</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
+        <v>1944</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="1"/>
+        <v>3402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="7">
         <v>917</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
+        <v>1834</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="1"/>
+        <v>3209.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="7">
         <v>866</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
+        <v>1732</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="1"/>
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="7">
         <v>827</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
+        <v>1654</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="1"/>
+        <v>2894.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="7">
         <v>797</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
+        <v>1594</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="1"/>
+        <v>2789.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="6">
+        <v>772</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="0"/>
+        <v>1544</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="1"/>
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="1">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="6">
+        <v>752</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="0"/>
+        <v>1504</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="1"/>
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="1">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="B34" s="6">
+        <v>733</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="0"/>
+        <v>1466</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="1"/>
+        <v>2565.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="1">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="B35" s="6">
+        <v>713</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="0"/>
+        <v>1426</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="1"/>
+        <v>2495.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="1">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="B36" s="6">
+        <v>695</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="0"/>
+        <v>1390</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="1"/>
+        <v>2432.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="1">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="B37" s="6">
+        <v>677</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" si="0"/>
+        <v>1354</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="1"/>
+        <v>2369.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B37" s="1">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="B38" s="6">
+        <v>659</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="0"/>
+        <v>1318</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="1"/>
+        <v>2306.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="1">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="B39" s="6">
+        <v>642</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="0"/>
+        <v>1284</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="1"/>
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B39" s="1">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="B40" s="6">
+        <v>625</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="1"/>
+        <v>2187.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="1">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="B41" s="6">
+        <v>609</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="0"/>
+        <v>1218</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="1"/>
+        <v>2131.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="1">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="B42" s="6">
+        <v>593</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="0"/>
+        <v>1186</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="1"/>
+        <v>2075.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="1">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="B43" s="6">
+        <v>577</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" si="0"/>
+        <v>1154</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="1"/>
+        <v>2019.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B43" s="1">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="B44" s="6">
+        <v>562</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="0"/>
+        <v>1124</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="1"/>
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45" s="6">
+        <v>548</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" si="0"/>
+        <v>1096</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="1"/>
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="6">
+        <v>533</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" si="0"/>
+        <v>1066</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="1"/>
+        <v>1865.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="6">
+        <v>520</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" si="0"/>
+        <v>1040</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="1"/>
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="6">
+        <v>506</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" si="0"/>
+        <v>1012</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="1"/>
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="6">
+        <v>493</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" si="0"/>
+        <v>986</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="1"/>
+        <v>1725.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50" s="6">
+        <v>480</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="1"/>
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="6">
+        <v>468</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" si="0"/>
+        <v>936</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="1"/>
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="6">
+        <v>455</v>
+      </c>
+      <c r="C52" s="7">
+        <f t="shared" si="0"/>
+        <v>910</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="1"/>
+        <v>1592.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B53" s="6">
+        <v>444</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="0"/>
+        <v>888</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="1"/>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="6">
+        <v>433</v>
+      </c>
+      <c r="C54" s="7">
+        <f t="shared" si="0"/>
+        <v>866</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="1"/>
+        <v>1515.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="6">
+        <v>424</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="0"/>
+        <v>848</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="1"/>
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="6">
+        <v>414</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="0"/>
+        <v>828</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="1"/>
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="6">
+        <v>406</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" si="0"/>
+        <v>812</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="1"/>
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" s="6">
+        <v>397</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" si="0"/>
+        <v>794</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="1"/>
+        <v>1389.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="6">
+        <v>388</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" si="0"/>
+        <v>776</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="1"/>
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="6">
+        <v>382</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="0"/>
+        <v>764</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="1"/>
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="6">
+        <v>377</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="0"/>
+        <v>754</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="1"/>
+        <v>1319.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="6">
+        <v>372</v>
+      </c>
+      <c r="C62" s="7">
+        <f t="shared" si="0"/>
+        <v>744</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="1"/>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="6">
+        <v>367</v>
+      </c>
+      <c r="C63" s="7">
+        <f t="shared" si="0"/>
+        <v>734</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="1"/>
+        <v>1284.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" s="6">
+        <v>362</v>
+      </c>
+      <c r="C64" s="7">
+        <f t="shared" si="0"/>
+        <v>724</v>
+      </c>
+      <c r="D64" s="7">
+        <f t="shared" si="1"/>
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" s="6">
+        <v>357</v>
+      </c>
+      <c r="C65" s="7">
+        <f t="shared" si="0"/>
+        <v>714</v>
+      </c>
+      <c r="D65" s="7">
+        <f t="shared" si="1"/>
+        <v>1249.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" s="6">
+        <v>353</v>
+      </c>
+      <c r="C66" s="7">
+        <f t="shared" si="0"/>
+        <v>706</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="1"/>
+        <v>1235.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B67" s="6">
+        <v>348</v>
+      </c>
+      <c r="C67" s="7">
+        <f t="shared" ref="C67:C121" si="2">B67*2</f>
+        <v>696</v>
+      </c>
+      <c r="D67" s="7">
+        <f t="shared" ref="D67:D121" si="3">B67*3.5</f>
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B68" s="6">
+        <v>344</v>
+      </c>
+      <c r="C68" s="7">
+        <f t="shared" si="2"/>
+        <v>688</v>
+      </c>
+      <c r="D68" s="7">
+        <f t="shared" si="3"/>
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B69" s="6">
+        <v>339</v>
+      </c>
+      <c r="C69" s="7">
+        <f t="shared" si="2"/>
+        <v>678</v>
+      </c>
+      <c r="D69" s="7">
+        <f t="shared" si="3"/>
+        <v>1186.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B70" s="6">
+        <v>335</v>
+      </c>
+      <c r="C70" s="7">
+        <f t="shared" si="2"/>
+        <v>670</v>
+      </c>
+      <c r="D70" s="7">
+        <f t="shared" si="3"/>
+        <v>1172.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" s="6">
+        <v>331</v>
+      </c>
+      <c r="C71" s="7">
+        <f t="shared" si="2"/>
+        <v>662</v>
+      </c>
+      <c r="D71" s="7">
+        <f t="shared" si="3"/>
+        <v>1158.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B72" s="6">
+        <v>326</v>
+      </c>
+      <c r="C72" s="7">
+        <f t="shared" si="2"/>
+        <v>652</v>
+      </c>
+      <c r="D72" s="7">
+        <f t="shared" si="3"/>
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="6">
+        <v>322</v>
+      </c>
+      <c r="C73" s="7">
+        <f t="shared" si="2"/>
+        <v>644</v>
+      </c>
+      <c r="D73" s="7">
+        <f t="shared" si="3"/>
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" s="6">
+        <v>318</v>
+      </c>
+      <c r="C74" s="7">
+        <f t="shared" si="2"/>
+        <v>636</v>
+      </c>
+      <c r="D74" s="7">
+        <f t="shared" si="3"/>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B75" s="6">
+        <v>314</v>
+      </c>
+      <c r="C75" s="7">
+        <f t="shared" si="2"/>
+        <v>628</v>
+      </c>
+      <c r="D75" s="7">
+        <f t="shared" si="3"/>
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B76" s="6">
+        <v>310</v>
+      </c>
+      <c r="C76" s="7">
+        <f t="shared" si="2"/>
+        <v>620</v>
+      </c>
+      <c r="D76" s="7">
+        <f t="shared" si="3"/>
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" s="6">
+        <v>306</v>
+      </c>
+      <c r="C77" s="7">
+        <f t="shared" si="2"/>
+        <v>612</v>
+      </c>
+      <c r="D77" s="7">
+        <f t="shared" si="3"/>
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B78" s="6">
+        <v>303</v>
+      </c>
+      <c r="C78" s="7">
+        <f t="shared" si="2"/>
+        <v>606</v>
+      </c>
+      <c r="D78" s="7">
+        <f t="shared" si="3"/>
+        <v>1060.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B79" s="6">
+        <v>299</v>
+      </c>
+      <c r="C79" s="7">
+        <f t="shared" si="2"/>
+        <v>598</v>
+      </c>
+      <c r="D79" s="7">
+        <f t="shared" si="3"/>
+        <v>1046.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" s="6">
+        <v>295</v>
+      </c>
+      <c r="C80" s="7">
+        <f t="shared" si="2"/>
+        <v>590</v>
+      </c>
+      <c r="D80" s="7">
+        <f t="shared" si="3"/>
+        <v>1032.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" s="6">
+        <v>292</v>
+      </c>
+      <c r="C81" s="7">
+        <f t="shared" si="2"/>
+        <v>584</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" si="3"/>
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B82" s="6">
+        <v>288</v>
+      </c>
+      <c r="C82" s="7">
+        <f t="shared" si="2"/>
+        <v>576</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="3"/>
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B83" s="6">
+        <v>284</v>
+      </c>
+      <c r="C83" s="7">
+        <f t="shared" si="2"/>
+        <v>568</v>
+      </c>
+      <c r="D83" s="7">
+        <f t="shared" si="3"/>
+        <v>994</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" s="6">
+        <v>281</v>
+      </c>
+      <c r="C84" s="7">
+        <f t="shared" si="2"/>
         <v>562</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="1">
+      <c r="D84" s="7">
+        <f t="shared" si="3"/>
+        <v>983.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B85" s="6">
+        <v>278</v>
+      </c>
+      <c r="C85" s="7">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+      <c r="D85" s="7">
+        <f t="shared" si="3"/>
+        <v>973</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" s="6">
+        <v>274</v>
+      </c>
+      <c r="C86" s="7">
+        <f t="shared" si="2"/>
         <v>548</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" s="1">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="1">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" s="1">
+      <c r="D86" s="7">
+        <f t="shared" si="3"/>
+        <v>959</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="6">
+        <v>271</v>
+      </c>
+      <c r="C87" s="7">
+        <f t="shared" si="2"/>
+        <v>542</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" si="3"/>
+        <v>948.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="6">
+        <v>268</v>
+      </c>
+      <c r="C88" s="7">
+        <f t="shared" si="2"/>
+        <v>536</v>
+      </c>
+      <c r="D88" s="7">
+        <f t="shared" si="3"/>
+        <v>938</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="6">
+        <v>264</v>
+      </c>
+      <c r="C89" s="7">
+        <f t="shared" si="2"/>
+        <v>528</v>
+      </c>
+      <c r="D89" s="7">
+        <f t="shared" si="3"/>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" s="6">
+        <v>261</v>
+      </c>
+      <c r="C90" s="7">
+        <f t="shared" si="2"/>
+        <v>522</v>
+      </c>
+      <c r="D90" s="7">
+        <f t="shared" si="3"/>
+        <v>913.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B91" s="6">
+        <v>258</v>
+      </c>
+      <c r="C91" s="7">
+        <f t="shared" si="2"/>
+        <v>516</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" si="3"/>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="6">
+        <v>256</v>
+      </c>
+      <c r="C92" s="7">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="3"/>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="6">
+        <v>253</v>
+      </c>
+      <c r="C93" s="7">
+        <f t="shared" si="2"/>
         <v>506</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B49" s="1">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B50" s="1">
+      <c r="D93" s="7">
+        <f t="shared" si="3"/>
+        <v>885.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" s="6">
+        <v>251</v>
+      </c>
+      <c r="C94" s="7">
+        <f t="shared" si="2"/>
+        <v>502</v>
+      </c>
+      <c r="D94" s="7">
+        <f t="shared" si="3"/>
+        <v>878.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" s="6">
+        <v>249</v>
+      </c>
+      <c r="C95" s="7">
+        <f t="shared" si="2"/>
+        <v>498</v>
+      </c>
+      <c r="D95" s="7">
+        <f t="shared" si="3"/>
+        <v>871.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="6">
+        <v>247</v>
+      </c>
+      <c r="C96" s="7">
+        <f t="shared" si="2"/>
+        <v>494</v>
+      </c>
+      <c r="D96" s="7">
+        <f t="shared" si="3"/>
+        <v>864.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B97" s="6">
+        <v>245</v>
+      </c>
+      <c r="C97" s="7">
+        <f t="shared" si="2"/>
+        <v>490</v>
+      </c>
+      <c r="D97" s="7">
+        <f t="shared" si="3"/>
+        <v>857.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="6">
+        <v>242</v>
+      </c>
+      <c r="C98" s="7">
+        <f t="shared" si="2"/>
+        <v>484</v>
+      </c>
+      <c r="D98" s="7">
+        <f t="shared" si="3"/>
+        <v>847</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="6">
+        <v>240</v>
+      </c>
+      <c r="C99" s="7">
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B51" s="1">
+      <c r="D99" s="7">
+        <f t="shared" si="3"/>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B100" s="6">
+        <v>238</v>
+      </c>
+      <c r="C100" s="7">
+        <f t="shared" si="2"/>
+        <v>476</v>
+      </c>
+      <c r="D100" s="7">
+        <f t="shared" si="3"/>
+        <v>833</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" s="6">
+        <v>236</v>
+      </c>
+      <c r="C101" s="7">
+        <f t="shared" si="2"/>
+        <v>472</v>
+      </c>
+      <c r="D101" s="7">
+        <f t="shared" si="3"/>
+        <v>826</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B102" s="6">
+        <v>234</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" si="2"/>
         <v>468</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B52" s="1">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B53" s="1">
+      <c r="D102" s="7">
+        <f t="shared" si="3"/>
+        <v>819</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B103" s="6">
+        <v>232</v>
+      </c>
+      <c r="C103" s="7">
+        <f t="shared" si="2"/>
+        <v>464</v>
+      </c>
+      <c r="D103" s="7">
+        <f t="shared" si="3"/>
+        <v>812</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B104" s="6">
+        <v>230</v>
+      </c>
+      <c r="C104" s="7">
+        <f t="shared" si="2"/>
+        <v>460</v>
+      </c>
+      <c r="D104" s="7">
+        <f t="shared" si="3"/>
+        <v>805</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" s="6">
+        <v>228</v>
+      </c>
+      <c r="C105" s="7">
+        <f t="shared" si="2"/>
+        <v>456</v>
+      </c>
+      <c r="D105" s="7">
+        <f t="shared" si="3"/>
+        <v>798</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B106" s="6">
+        <v>226</v>
+      </c>
+      <c r="C106" s="7">
+        <f t="shared" si="2"/>
+        <v>452</v>
+      </c>
+      <c r="D106" s="7">
+        <f t="shared" si="3"/>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" s="6">
+        <v>224</v>
+      </c>
+      <c r="C107" s="7">
+        <f t="shared" si="2"/>
+        <v>448</v>
+      </c>
+      <c r="D107" s="7">
+        <f t="shared" si="3"/>
+        <v>784</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B108" s="6">
+        <v>222</v>
+      </c>
+      <c r="C108" s="7">
+        <f t="shared" si="2"/>
         <v>444</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B54" s="1">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B55" s="1">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B56" s="1">
+      <c r="D108" s="7">
+        <f t="shared" si="3"/>
+        <v>777</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B109" s="6">
+        <v>220</v>
+      </c>
+      <c r="C109" s="7">
+        <f t="shared" si="2"/>
+        <v>440</v>
+      </c>
+      <c r="D109" s="7">
+        <f t="shared" si="3"/>
+        <v>770</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B110" s="6">
+        <v>218</v>
+      </c>
+      <c r="C110" s="7">
+        <f t="shared" si="2"/>
+        <v>436</v>
+      </c>
+      <c r="D110" s="7">
+        <f t="shared" si="3"/>
+        <v>763</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B111" s="6">
+        <v>216</v>
+      </c>
+      <c r="C111" s="7">
+        <f t="shared" si="2"/>
+        <v>432</v>
+      </c>
+      <c r="D111" s="7">
+        <f t="shared" si="3"/>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B112" s="6">
+        <v>214</v>
+      </c>
+      <c r="C112" s="7">
+        <f t="shared" si="2"/>
+        <v>428</v>
+      </c>
+      <c r="D112" s="7">
+        <f t="shared" si="3"/>
+        <v>749</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B113" s="6">
+        <v>213</v>
+      </c>
+      <c r="C113" s="7">
+        <f t="shared" si="2"/>
+        <v>426</v>
+      </c>
+      <c r="D113" s="7">
+        <f t="shared" si="3"/>
+        <v>745.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B114" s="6">
+        <v>211</v>
+      </c>
+      <c r="C114" s="7">
+        <f t="shared" si="2"/>
+        <v>422</v>
+      </c>
+      <c r="D114" s="7">
+        <f t="shared" si="3"/>
+        <v>738.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B115" s="6">
+        <v>209</v>
+      </c>
+      <c r="C115" s="7">
+        <f t="shared" si="2"/>
+        <v>418</v>
+      </c>
+      <c r="D115" s="7">
+        <f t="shared" si="3"/>
+        <v>731.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B116" s="6">
+        <v>207</v>
+      </c>
+      <c r="C116" s="7">
+        <f t="shared" si="2"/>
         <v>414</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B57" s="1">
+      <c r="D116" s="7">
+        <f t="shared" si="3"/>
+        <v>724.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" s="6">
+        <v>205</v>
+      </c>
+      <c r="C117" s="7">
+        <f t="shared" si="2"/>
+        <v>410</v>
+      </c>
+      <c r="D117" s="7">
+        <f t="shared" si="3"/>
+        <v>717.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B118" s="6">
+        <v>203</v>
+      </c>
+      <c r="C118" s="7">
+        <f t="shared" si="2"/>
         <v>406</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B58" s="1">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B59" s="1">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" s="1">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B61" s="1">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62" s="1">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B63" s="1">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B64" s="1">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" s="1">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B66" s="1">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B67" s="1">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" s="1">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B69" s="1">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B70" s="1">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B71" s="1">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B72" s="1">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B73" s="1">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B74" s="1">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B75" s="1">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B76" s="1">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B77" s="1">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B78" s="1">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B79" s="1">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B80" s="1">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B81" s="1">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B82" s="1">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B83" s="1">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B84" s="1">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B85" s="1">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B86" s="1">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B87" s="1">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B88" s="1">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B89" s="1">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B90" s="1">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B91" s="1">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B92" s="1">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B93" s="1">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B94" s="1">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B95" s="1">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B96" s="1">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B97" s="1">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B98" s="1">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B99" s="1">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B100" s="1">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B101" s="1">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" s="1">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B103" s="1">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B104" s="1">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B105" s="1">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B106" s="1">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="7" t="s">
+      <c r="D118" s="7">
+        <f t="shared" si="3"/>
+        <v>710.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B119" s="6">
+        <v>202</v>
+      </c>
+      <c r="C119" s="7">
+        <f t="shared" si="2"/>
+        <v>404</v>
+      </c>
+      <c r="D119" s="7">
+        <f t="shared" si="3"/>
+        <v>707</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B120" s="6">
+        <v>200</v>
+      </c>
+      <c r="C120" s="7">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="D120" s="7">
+        <f t="shared" si="3"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B121" s="6">
         <v>198</v>
       </c>
-      <c r="B107" s="1">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B108" s="1">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B109" s="1">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B110" s="1">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B111" s="1">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B112" s="1">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="B113" s="1">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B114" s="1">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B115" s="1">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="B116" s="1">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B117" s="1">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B118" s="1">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B119" s="1">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="B120" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B121" s="1">
-        <v>198</v>
+      <c r="C121" s="7">
+        <f t="shared" si="2"/>
+        <v>396</v>
+      </c>
+      <c r="D121" s="7">
+        <f t="shared" si="3"/>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4919,14 +5893,14 @@
         <v>77</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2" s="6">
         <f>0.1/12</f>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5229,7 +6203,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7">
         <v>1.7236</v>
@@ -5246,7 +6220,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="7">
         <v>1.7236</v>
@@ -5254,7 +6228,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="7">
         <v>1.7236</v>
@@ -5262,7 +6236,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="7">
         <v>1.7236</v>
@@ -5270,7 +6244,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="7">
         <v>1.7236</v>
@@ -5278,7 +6252,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7">
         <v>1.7236</v>
@@ -5286,7 +6260,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="7">
         <v>1.7236</v>
@@ -5294,7 +6268,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="7">
         <v>1.7236</v>
@@ -5302,7 +6276,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="7">
         <v>1.7236</v>
@@ -5310,7 +6284,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="7">
         <v>1.7236</v>
@@ -5318,7 +6292,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="7">
         <v>1.7236</v>
@@ -5326,7 +6300,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="7">
         <v>1.7236</v>
@@ -5334,7 +6308,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="7">
         <v>1.7236</v>
@@ -5342,7 +6316,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="7">
         <v>1.7236</v>
@@ -5350,7 +6324,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="7">
         <v>1.7236</v>
@@ -5358,7 +6332,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="7">
         <v>1.7236</v>
@@ -5366,7 +6340,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="7">
         <v>1.7236</v>
@@ -5374,7 +6348,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="7">
         <v>1.7236</v>
@@ -5382,7 +6356,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="7">
         <v>1.7236</v>
@@ -5390,7 +6364,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="7">
         <v>1.7236</v>
@@ -5398,7 +6372,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="7">
         <v>1.7236</v>
@@ -5406,7 +6380,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="7">
         <v>1.7236</v>
@@ -5414,7 +6388,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="7">
         <v>1.7236</v>
@@ -5422,7 +6396,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="7">
         <v>1.7236</v>
@@ -5430,7 +6404,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="7">
         <v>1.7236</v>
@@ -5438,7 +6412,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="7">
         <v>1.7236</v>
@@ -5446,7 +6420,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="7">
         <v>1.7236</v>
@@ -5454,7 +6428,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="7">
         <v>1.7236</v>
@@ -5462,7 +6436,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" s="7">
         <v>1.7236</v>
@@ -5470,7 +6444,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="7">
         <v>1.7236</v>
@@ -5478,7 +6452,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="7">
         <v>1.7236</v>
@@ -5486,7 +6460,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="7">
         <v>1.7236</v>
@@ -5494,7 +6468,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="7">
         <v>1.7236</v>
@@ -5502,7 +6476,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="7">
         <v>1.7236</v>
@@ -5510,7 +6484,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37" s="7">
         <v>1.7236</v>
@@ -5518,7 +6492,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="7">
         <v>1.7236</v>
@@ -5526,7 +6500,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39" s="7">
         <v>1.7236</v>
@@ -5534,7 +6508,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="7">
         <v>1.7236</v>
@@ -5542,7 +6516,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" s="7">
         <v>1.7236</v>
@@ -5550,7 +6524,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="7">
         <v>1.7236</v>
@@ -5558,7 +6532,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="7">
         <v>1.7236</v>
@@ -5566,7 +6540,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="7">
         <v>1.7236</v>
@@ -5574,7 +6548,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="7">
         <v>1.7236</v>
@@ -5582,7 +6556,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="7">
         <v>1.7236</v>
@@ -5590,7 +6564,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="7">
         <v>1.7236</v>
@@ -5598,7 +6572,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B48" s="7">
         <v>1.7236</v>
@@ -5606,7 +6580,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B49" s="7">
         <v>1.7236</v>
@@ -5614,7 +6588,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="7">
         <v>1.7236</v>
@@ -5622,7 +6596,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B51" s="7">
         <v>1.7236</v>
@@ -5630,7 +6604,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B52" s="7">
         <v>1.7236</v>
@@ -5638,7 +6612,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53" s="7">
         <v>1.7236</v>
@@ -5646,7 +6620,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="7">
         <v>1.7236</v>
@@ -5654,7 +6628,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B55" s="7">
         <v>1.7236</v>
@@ -5662,7 +6636,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B56" s="7">
         <v>1.7236</v>
@@ -5670,7 +6644,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57" s="7">
         <v>1.7236</v>
@@ -5678,7 +6652,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" s="7">
         <v>1.7236</v>
@@ -5686,7 +6660,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="7">
         <v>1.7236</v>
@@ -5694,7 +6668,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B60" s="7">
         <v>1.7236</v>
@@ -5702,7 +6676,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" s="7">
         <v>1.7236</v>
@@ -5710,7 +6684,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62" s="7">
         <v>1.7236</v>
@@ -5718,7 +6692,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" s="7">
         <v>1.7236</v>
@@ -5726,7 +6700,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B64" s="7">
         <v>1.7236</v>
@@ -5734,7 +6708,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" s="7">
         <v>1.7236</v>
@@ -5742,7 +6716,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B66" s="7">
         <v>1.7236</v>
@@ -5750,7 +6724,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B67" s="7">
         <v>1.7236</v>
@@ -5758,7 +6732,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" s="7">
         <v>1.7236</v>
@@ -5766,7 +6740,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B69" s="7">
         <v>1.7236</v>
@@ -5774,7 +6748,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B70" s="7">
         <v>1.7236</v>
@@ -5782,7 +6756,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71" s="7">
         <v>1.7236</v>
@@ -5790,7 +6764,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B72" s="7">
         <v>1.7236</v>
@@ -5798,7 +6772,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" s="7">
         <v>1.7236</v>
@@ -5806,7 +6780,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74" s="7">
         <v>1.7236</v>
@@ -5814,7 +6788,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" s="7">
         <v>1.7236</v>
@@ -5822,7 +6796,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76" s="7">
         <v>1.7236</v>
@@ -5830,7 +6804,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" s="7">
         <v>1.7236</v>
@@ -5838,7 +6812,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" s="7">
         <v>1.7236</v>
@@ -5846,7 +6820,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="7">
         <v>1.7236</v>
@@ -5854,7 +6828,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" s="7">
         <v>1.7236</v>
@@ -5862,7 +6836,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="7">
         <v>1.7236</v>
@@ -5870,7 +6844,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B82" s="7">
         <v>1.7236</v>
@@ -5878,7 +6852,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B83" s="7">
         <v>1.7236</v>
@@ -5886,7 +6860,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" s="7">
         <v>1.7236</v>
@@ -5894,7 +6868,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7">
         <v>1.7236</v>
@@ -5902,7 +6876,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B86" s="7">
         <v>1.7236</v>
@@ -5910,7 +6884,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B87" s="7">
         <v>1.7236</v>
@@ -5918,7 +6892,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88" s="7">
         <v>1.7236</v>
@@ -5926,7 +6900,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B89" s="7">
         <v>1.7236</v>
@@ -5934,7 +6908,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B90" s="7">
         <v>1.7236</v>
@@ -5942,7 +6916,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" s="7">
         <v>1.7236</v>
@@ -5950,7 +6924,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92" s="7">
         <v>1.7236</v>
@@ -5958,7 +6932,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" s="7">
         <v>1.7236</v>
@@ -5966,7 +6940,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B94" s="7">
         <v>1.7236</v>
@@ -5974,7 +6948,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95" s="7">
         <v>1.7236</v>
@@ -5982,7 +6956,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96" s="7">
         <v>1.7236</v>
@@ -5990,7 +6964,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B97" s="7">
         <v>1.7236</v>
@@ -5998,7 +6972,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B98" s="7">
         <v>1.7236</v>
@@ -6006,7 +6980,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99" s="7">
         <v>1.7236</v>
@@ -6014,7 +6988,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B100" s="7">
         <v>1.7236</v>
@@ -6022,7 +6996,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B101" s="7">
         <v>1.7236</v>
@@ -6030,7 +7004,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B102" s="7">
         <v>1.7236</v>
@@ -6038,7 +7012,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B103" s="7">
         <v>1.7236</v>
@@ -6046,7 +7020,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B104" s="7">
         <v>1.7236</v>
@@ -6054,7 +7028,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B105" s="7">
         <v>1.7236</v>
@@ -6062,7 +7036,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B106" s="7">
         <v>1.7236</v>
@@ -6070,7 +7044,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B107" s="7">
         <v>1.7236</v>
@@ -6078,7 +7052,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B108" s="7">
         <v>1.7236</v>
@@ -6086,7 +7060,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B109" s="7">
         <v>1.7236</v>
@@ -6094,7 +7068,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B110" s="7">
         <v>1.7236</v>
@@ -6102,7 +7076,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B111" s="7">
         <v>1.7236</v>
@@ -6110,7 +7084,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" s="7">
         <v>1.7236</v>
@@ -6118,7 +7092,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B113" s="7">
         <v>1.7236</v>
@@ -6126,7 +7100,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B114" s="7">
         <v>1.7236</v>
@@ -6134,7 +7108,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B115" s="7">
         <v>1.7236</v>
@@ -6142,7 +7116,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B116" s="7">
         <v>1.7236</v>
@@ -6150,7 +7124,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B117" s="7">
         <v>1.7236</v>
@@ -6158,7 +7132,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B118" s="7">
         <v>1.7236</v>
@@ -6166,7 +7140,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B119" s="7">
         <v>1.7236</v>
@@ -6174,7 +7148,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B120" s="7">
         <v>1.7236</v>
@@ -6182,7 +7156,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B121" s="7">
         <v>1.7236</v>
@@ -6190,7 +7164,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B122" s="7">
         <v>1.7236</v>

</xml_diff>